<commit_message>
Fix reduce COLA/Chain CPI COLA
</commit_message>
<xml_diff>
--- a/options_guide.xlsx
+++ b/options_guide.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dynasim-shiny3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -94,12 +99,6 @@
     <t>13.4% Payroll Tax</t>
   </si>
   <si>
-    <t>Full Chained-CPI COLA</t>
-  </si>
-  <si>
-    <t>Partial Chained-CPI COLA</t>
-  </si>
-  <si>
     <t>Increase FRA</t>
   </si>
   <si>
@@ -124,12 +123,6 @@
     <t>BPC Package</t>
   </si>
   <si>
-    <t>BPCtableShellsEquivalentOPT1.xlsx</t>
-  </si>
-  <si>
-    <t>BPCtableShellsOPT1.xlsx</t>
-  </si>
-  <si>
     <t>BPCtableShellsEquivalentOPT2.xlsx</t>
   </si>
   <si>
@@ -139,9 +132,6 @@
     <t>BPCtableShellsEquivalentOPT3.xlsx</t>
   </si>
   <si>
-    <t>BPCtableShellsOPT3.xlsx</t>
-  </si>
-  <si>
     <t>BPCtableShellsEquivalentOPT4.xlsx</t>
   </si>
   <si>
@@ -226,18 +216,9 @@
     <t>BPCtableShellsRun5SaveOpt4withSUPERTAX.xlsx</t>
   </si>
   <si>
-    <t>BPCtableShellsEquivalentOPT0.xlsx</t>
-  </si>
-  <si>
     <t>BPCtableShellsOPT0.xlsx</t>
   </si>
   <si>
-    <t>BPCtableShellsEquivalentPayableV3.xlsx</t>
-  </si>
-  <si>
-    <t>BPCtableShellsPayableV3.xlsx</t>
-  </si>
-  <si>
     <t>option.name</t>
   </si>
   <si>
@@ -280,9 +261,6 @@
     <t>X:\programs\run912\opt8(increaseFRAERA)\</t>
   </si>
   <si>
-    <t>X:\programs\run912\opt12\</t>
-  </si>
-  <si>
     <t>X:\programs\run912\taxmax180000\</t>
   </si>
   <si>
@@ -317,12 +295,39 @@
   </si>
   <si>
     <t>X:\programs\run912\opt3(capSpouse)\</t>
+  </si>
+  <si>
+    <t>BPCtableShellsEquivalentMiniPIA.xlsx</t>
+  </si>
+  <si>
+    <t>BPCtableShellsMiniPIA.xlsx</t>
+  </si>
+  <si>
+    <t>BPCtableShellsCapSpouse.xlsx</t>
+  </si>
+  <si>
+    <t>BPCtableShellsEQOPT0.xlsx</t>
+  </si>
+  <si>
+    <t>BPCtableShellsPayable.xlsx</t>
+  </si>
+  <si>
+    <t>BPCtableShellsEquivalentPayable.xlsx</t>
+  </si>
+  <si>
+    <t>X:\programs\run912\opt12(taxmax150000)\</t>
+  </si>
+  <si>
+    <t>Reduce COLA</t>
+  </si>
+  <si>
+    <t>Chained-CPI COLA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,6 +379,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -421,7 +429,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -454,9 +462,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -489,6 +514,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -667,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,22 +726,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -711,17 +753,17 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE(E2,F2)</f>
         <v>X:\programs\run912\opt0\BPCtableShellsOPT0.xlsx</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -732,17 +774,17 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D39" si="0">CONCATENATE(E3,F3)</f>
-        <v>X:\programs\run912\opt0\BPCtableShellsEquivalentOPT0.xlsx</v>
+        <v>X:\programs\run912\opt0\BPCtableShellsEQOPT0.xlsx</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -754,17 +796,17 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>X:\programs\run912\payable\BPCtableShellsPayableV3.xlsx</v>
+        <v>X:\programs\run912\payable\BPCtableShellsPayable.xlsx</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -776,17 +818,17 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>X:\programs\run912\payable\BPCtableShellsEquivalentPayableV3.xlsx</v>
+        <v>X:\programs\run912\payable\BPCtableShellsEquivalentPayable.xlsx</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -798,17 +840,17 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>X:\programs\run912\opt1(MiniPIA)\BPCtableShellsOPT1.xlsx</v>
+        <v>X:\programs\run912\opt1(MiniPIA)\BPCtableShellsMiniPIA.xlsx</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -819,17 +861,17 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>X:\programs\run912\opt1(MiniPIA)\BPCtableShellsEquivalentOPT1.xlsx</v>
+        <v>X:\programs\run912\opt1(MiniPIA)\BPCtableShellsEquivalentMiniPIA.xlsx</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -840,17 +882,17 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt2(increaseTaxSSB)\BPCtableShellsOPT2.xlsx</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -861,17 +903,17 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt2(increaseTaxSSB)\BPCtableShellsEquivalentOPT2.xlsx</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -882,17 +924,17 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>X:\programs\run912\opt3(capSpouse)\BPCtableShellsOPT3.xlsx</v>
+        <v>X:\programs\run912\opt3(capSpouse)\BPCtableShellsCapSpouse.xlsx</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -903,17 +945,17 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt3(capSpouse)\BPCtableShellsEquivalentOPT3.xlsx</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -924,17 +966,17 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt4(survivorjs75)\BPCtableShellsOPT4.xlsx</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -945,17 +987,17 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt4(survivorjs75)\BPCtableShellsEquivalentOPT4.xlsx</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -966,17 +1008,17 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt5(increaseTAXMAX)\BPCtableShellsOPT5.xlsx</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -987,17 +1029,17 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt5(increaseTAXMAX)\BPCtableShellsEquivalentOPT5.xlsx</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F15" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1008,17 +1050,17 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt5B(RaiseFICA)\BPCtableShellsOPT5B.xlsx</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1029,17 +1071,17 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt5B(RaiseFICA)\BPCtableShellsEquivalentOPT5b.xlsx</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1050,17 +1092,17 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt5c(RaiseFICAonly)\BPCtableShellsOPT5c.xlsx</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1071,17 +1113,17 @@
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt5c(RaiseFICAonly)\BPCtableShellsEquivalentOPT5c.xlsx</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1089,20 +1131,20 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\ChainCPI\BPCtableShellsChainCPI.xlsx</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1110,20 +1152,20 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\ChainCPI\BPCtableShellsEquivalentChainCPI.xlsx</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1131,20 +1173,20 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt6(decreaseCOLA)\BPCtableShellsOPT6.xlsx</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1152,20 +1194,20 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt6(decreaseCOLA)\BPCtableShellsEquivalentOPT6.xlsx</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F23" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1173,20 +1215,20 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt7(IncreaseFRA)\BPCtableShellsOPT7.xlsx</v>
       </c>
       <c r="E24" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F24" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1194,20 +1236,20 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt7(IncreaseFRA)\BPCtableShellsEquivalentOPT7.xlsx</v>
       </c>
       <c r="E25" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F25" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1215,20 +1257,20 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt8(increaseFRAERA)\BPCtableShellsOPT8.xlsx</v>
       </c>
       <c r="E26" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1236,20 +1278,20 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\opt8(increaseFRAERA)\BPCtableShellsEquivalentOPT8.xlsx</v>
       </c>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1257,20 +1299,20 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>X:\programs\run912\opt12\BPCtableShellsOPT12.xlsx</v>
+        <v>X:\programs\run912\opt12(taxmax150000)\BPCtableShellsOPT12.xlsx</v>
       </c>
       <c r="E28" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="F28" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1278,20 +1320,20 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>X:\programs\run912\opt12\BPCtableShellsEquivalentOPT12.xlsx</v>
+        <v>X:\programs\run912\opt12(taxmax150000)\BPCtableShellsEquivalentOPT12.xlsx</v>
       </c>
       <c r="E29" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="F29" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1299,20 +1341,20 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\taxmax180000\BPCtableShellsTaxmax180000.xlsx</v>
       </c>
       <c r="E30" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1320,20 +1362,20 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\taxmax180000\BPCtableShellsEquivalentTaxmax180000.xlsx</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F31" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,20 +1383,20 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\Notaxmax\BPCtableShellsNotaxmax.xlsx</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F32" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1362,20 +1404,20 @@
         <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\Notaxmax\BPCtableShellsEquivalentNotaxmax.xlsx</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F33" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1383,20 +1425,20 @@
         <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\FICA14\BPCtableShellsFICA14.xlsx</v>
       </c>
       <c r="E34" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F34" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1404,20 +1446,20 @@
         <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\FICA14\BPCtableShellsEquivalentFICA14.xlsx</v>
       </c>
       <c r="E35" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F35" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1425,20 +1467,20 @@
         <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\Fica15\BPCtableShellsFICA15.xlsx</v>
       </c>
       <c r="E36" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F36" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1446,62 +1488,62 @@
         <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\run912\Fica15\BPCtableShellsEquivalentFICA15.xlsx</v>
       </c>
       <c r="E37" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F37" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D38" t="str">
-        <f>CONCATENATE(E38,F38)</f>
+        <f t="shared" si="0"/>
         <v>X:\programs\Run912\run5SaveOpt4\BPCtableShellsRun5SaveOpt4withSUPERTAX.xlsx</v>
       </c>
       <c r="E38" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F38" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
         <v>X:\programs\Run912\run5SaveOpt4\BPCtableShellsEquivalentRun5SaveOpt4.xlsx</v>
       </c>
       <c r="E39" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F39" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>